<commit_message>
Event table and activity diagram
Changed Government Level Admin to Local Government Unit Admin
</commit_message>
<xml_diff>
--- a/Documentation/EVENT TABLE.xlsx
+++ b/Documentation/EVENT TABLE.xlsx
@@ -75,24 +75,6 @@
     <t>Identified supplies</t>
   </si>
   <si>
-    <t>New Government Level Admin details</t>
-  </si>
-  <si>
-    <t>Government Level Admin</t>
-  </si>
-  <si>
-    <t>Government Level Admin details</t>
-  </si>
-  <si>
-    <t>Notified Government Level Admin</t>
-  </si>
-  <si>
-    <t>Government Level Admin identifies needed supplies</t>
-  </si>
-  <si>
-    <t>Government Level Admin requests for supplies</t>
-  </si>
-  <si>
     <t>NDRRMC submits predicted disaster details</t>
   </si>
   <si>
@@ -120,10 +102,28 @@
     <t>New information of predicted disaster and areas</t>
   </si>
   <si>
-    <t>Government Level Admin creates an account</t>
-  </si>
-  <si>
-    <t>Government Level Admin receives advisory</t>
+    <t>Local Governmet Unit Admin creates an account</t>
+  </si>
+  <si>
+    <t>New Local Governmet Unit Admin details</t>
+  </si>
+  <si>
+    <t>Local Governmet Unit Admin</t>
+  </si>
+  <si>
+    <t>Local Governmet Unit Admin details</t>
+  </si>
+  <si>
+    <t>Local Governmet Unit Admin receives advisory</t>
+  </si>
+  <si>
+    <t>Notified Local Governmet Unit Admin</t>
+  </si>
+  <si>
+    <t>Local Governmet Unit Admin identifies needed supplies</t>
+  </si>
+  <si>
+    <t>Local Governmet Unit Admin requests for supplies</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
@@ -527,22 +527,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.35">
@@ -550,22 +550,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -573,22 +573,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -596,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>13</v>
@@ -608,10 +608,10 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -619,13 +619,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
@@ -634,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -642,13 +642,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>9</v>

</xml_diff>